<commit_message>
10 years battery replacement (b)
</commit_message>
<xml_diff>
--- a/Scenarios/b_Conventional-MicroGrid/Results/EnergySystemSize.xlsx
+++ b/Scenarios/b_Conventional-MicroGrid/Results/EnergySystemSize.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive\Documenti\GitHub\MicroGridsPy-MultiEnergy_Paper\Scenarios\b_Conventional-MicroGrid\Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260A5075-0C18-4C4E-B003-5A814CC67B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="17895" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Size" sheetId="1" r:id="rId1"/>
@@ -135,8 +129,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,7 +142,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,9 +196,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -495,23 +485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -554,10 +540,10 @@
         <v>9</v>
       </c>
       <c r="G2">
-        <v>1.026039438972418E-9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>320.37394354013549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -577,10 +563,10 @@
         <v>9</v>
       </c>
       <c r="G3">
-        <v>3.9647480732359968E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1620.946024170172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -600,10 +586,10 @@
         <v>9</v>
       </c>
       <c r="G4">
-        <v>169.89199208860009</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18.714822794742179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -611,19 +597,19 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>262.35290291666888</v>
+        <v>244.98844740528031</v>
       </c>
       <c r="D5">
-        <v>1157.1068498123971</v>
+        <v>1069.252757002477</v>
       </c>
       <c r="E5">
-        <v>40.191186936989567</v>
+        <v>54.722222994710577</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>47.442304286471263</v>
       </c>
       <c r="G5">
-        <v>1459.6509396660549</v>
+        <v>1416.4057316889391</v>
       </c>
     </row>
   </sheetData>
@@ -632,23 +618,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -677,7 +661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -703,10 +687,10 @@
         <v>9</v>
       </c>
       <c r="I2">
-        <v>0.28781392548887652</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.9840096059080814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -732,10 +716,10 @@
         <v>9</v>
       </c>
       <c r="I3">
-        <v>2.0520788779448361E-12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.64074788708027108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -759,10 +743,10 @@
         <v>9</v>
       </c>
       <c r="I4">
-        <v>2.1806114402797978E-8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.89152031329359449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -786,10 +770,10 @@
         <v>9</v>
       </c>
       <c r="I5">
-        <v>3.3978398417720032E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3.7429645589484349E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -801,22 +785,22 @@
         <v>17</v>
       </c>
       <c r="E6">
-        <v>2.623529029166689E-2</v>
+        <v>2.449884474052803E-2</v>
       </c>
       <c r="F6">
-        <v>0.11571068498123969</v>
+        <v>0.10692527570024769</v>
       </c>
       <c r="G6">
-        <v>4.0191186936989563E-3</v>
+        <v>5.4722222994710579E-3</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>4.7442304286471251E-3</v>
       </c>
       <c r="I6">
-        <v>0.14596509396660551</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.14164057316889389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -842,10 +826,10 @@
         <v>9</v>
       </c>
       <c r="I7">
-        <v>5.7288317321776757E-13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.1788789342984472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -869,10 +853,10 @@
         <v>9</v>
       </c>
       <c r="I8">
-        <v>6.0876587878218964E-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.24888759957377349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -896,10 +880,10 @@
         <v>9</v>
       </c>
       <c r="I9">
-        <v>4.7429104494014253E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.2246564126217391E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -911,22 +895,22 @@
         <v>17</v>
       </c>
       <c r="E10">
-        <v>5.4931208471498101E-3</v>
+        <v>5.1295454816456159E-3</v>
       </c>
       <c r="F10">
-        <v>2.4227396336846389E-2</v>
+        <v>2.2387915456869651E-2</v>
       </c>
       <c r="G10">
-        <v>8.4151935953762709E-4</v>
+        <v>1.1457688502501671E-3</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>9.9334258479928596E-4</v>
       </c>
       <c r="I10">
-        <v>3.056203654353383E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.965657237356472E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -952,10 +936,10 @@
         <v>9</v>
       </c>
       <c r="I11">
-        <v>1.05439456453275E-8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.61993146406142541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -981,10 +965,10 @@
         <v>9</v>
       </c>
       <c r="I12">
-        <v>1.0187500690442729E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.13939342809793881</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -996,22 +980,22 @@
         <v>17</v>
       </c>
       <c r="E13">
-        <v>4.9124523107544546E-3</v>
+        <v>1.9334535389604219</v>
       </c>
       <c r="F13">
-        <v>1.4564267703182129E-2</v>
+        <v>5.6675463408115663</v>
       </c>
       <c r="G13">
-        <v>2.1504346622544339E-4</v>
+        <v>8.2659900189235955E-2</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>2.0656897088802501E-2</v>
       </c>
       <c r="I13">
-        <v>1.9691763480162029E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7.7043166770500262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1040,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1080,19 +1064,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1103,7 +1087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1111,16 +1095,16 @@
         <v>29</v>
       </c>
       <c r="C2">
-        <v>7.1815920131183857</v>
+        <v>960.46647168614982</v>
       </c>
       <c r="D2">
-        <v>7.1234666050238884</v>
+        <v>2787.02527677542</v>
       </c>
       <c r="E2">
-        <v>14.305058618142271</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3747.4917484615698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1134,10 +1118,10 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <v>0.99999999999946998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.76992550822477179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1151,10 +1135,10 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>5.3009676652100733E-13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.23007449177522829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1162,16 +1146,16 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>0.29999886460613462</v>
+        <v>0.82901061634023565</v>
       </c>
       <c r="D5">
-        <v>0.87878759932021533</v>
+        <v>0.87878523447900447</v>
       </c>
       <c r="E5">
-        <v>0.58821734263955183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.86602820789371726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1185,7 +1169,7 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>2.4504300849003129</v>
+        <v>0.22038916861858751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>